<commit_message>
Major Changes - Stock Dumps Downloaded and code updated
</commit_message>
<xml_diff>
--- a/StockDumpsSource/Coal India.xlsx
+++ b/StockDumpsSource/Coal India.xlsx
@@ -4086,7 +4086,7 @@
         <v>43</v>
       </c>
       <c r="B8">
-        <v>147.40</v>
+        <v>148.75</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -4094,7 +4094,7 @@
         <v>80</v>
       </c>
       <c r="B9">
-        <v>90838.62</v>
+        <v>91670.58</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>